<commit_message>
add v2 led mappings
</commit_message>
<xml_diff>
--- a/hardware/led_register_mappings_v2.xlsx
+++ b/hardware/led_register_mappings_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\traffic-pcb-sb\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29270128-0DEB-4671-A4C6-CB7062728D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8517499B-0A54-473C-A7B8-42CFB2B597B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{54825337-5B42-4940-B27B-8F4016375D87}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{54825337-5B42-4940-B27B-8F4016375D87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1126,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC9F51E-505F-4752-A582-E5A633FBEC92}">
   <dimension ref="A1:AF198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI45" sqref="AI45"/>
+    <sheetView tabSelected="1" topLeftCell="I41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P79" sqref="P79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>